<commit_message>
Update Harness to PT Expansion
</commit_message>
<xml_diff>
--- a/SDGM_Pins.xlsx
+++ b/SDGM_Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettpall/Documents/GitHub/GMSDGMConnector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64480B2-13B2-1F4D-B992-BD51FC0E024F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE77FBA-35C6-B947-B914-987F8C4D62D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11260" windowHeight="18420" xr2:uid="{2773CD03-8BBC-B349-81A9-5A6BBE33454F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33580" windowHeight="18420" xr2:uid="{2773CD03-8BBC-B349-81A9-5A6BBE33454F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="74">
   <si>
     <t>X1-1</t>
   </si>
@@ -255,12 +255,6 @@
     <t>GROUND</t>
   </si>
   <si>
-    <t>CAN +</t>
-  </si>
-  <si>
-    <t>CAN -</t>
-  </si>
-  <si>
     <t>Combined</t>
   </si>
   <si>
@@ -271,6 +265,21 @@
   </si>
   <si>
     <t>2019 Enclave</t>
+  </si>
+  <si>
+    <t>2022 Traverse</t>
+  </si>
+  <si>
+    <t>PT CAN +</t>
+  </si>
+  <si>
+    <t>PT CAN -</t>
+  </si>
+  <si>
+    <t>Object CAN +</t>
+  </si>
+  <si>
+    <t>Object CAN -</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +326,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -330,11 +345,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,22 +685,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C00BB16-2E14-714F-9E48-7A57C8D3D840}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -693,16 +713,19 @@
         <v>61</v>
       </c>
       <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -724,18 +747,21 @@
       <c r="G2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -758,8 +784,11 @@
       <c r="G5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -782,8 +811,11 @@
       <c r="G6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -792,7 +824,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -814,8 +846,11 @@
       <c r="G8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -838,8 +873,11 @@
       <c r="G9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -862,8 +900,11 @@
       <c r="G10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -871,14 +912,17 @@
         <f t="array" ref="B11">IF(OR(IF(C11:Z11="X",1,0)),"X","")</f>
         <v>X</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -887,7 +931,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -896,7 +940,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -919,8 +963,11 @@
       <c r="G14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -943,8 +990,11 @@
       <c r="G15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -967,8 +1017,11 @@
       <c r="G16" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -991,8 +1044,11 @@
       <c r="G17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1015,8 +1071,11 @@
       <c r="G18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1039,8 +1098,11 @@
       <c r="G19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1048,14 +1110,17 @@
         <f t="array" ref="B20">IF(OR(IF(C20:Z20="X",1,0)),"X","")</f>
         <v>X</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1073,7 +1138,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1082,7 +1147,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1156,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1100,7 +1165,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1174,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1118,7 +1183,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1141,8 +1206,11 @@
       <c r="G27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1219,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1160,7 +1228,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1169,7 +1237,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1192,8 +1260,11 @@
       <c r="G31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1211,149 +1282,165 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="str" cm="1">
-        <f t="array" ref="B33">IF(OR(IF(C33:Z33="X",1,0)),"X","")</f>
-        <v>X</v>
+      <c r="B33" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="H33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="str" cm="1">
-        <f t="array" ref="B34">IF(OR(IF(C34:Z34="X",1,0)),"X","")</f>
-        <v>X</v>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="H34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>65</v>
+      <c r="B35" t="str" cm="1">
+        <f t="array" ref="B35">IF(OR(IF(C35:Z35="X",1,0)),"X","")</f>
+        <v>X</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="H35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>66</v>
+      <c r="B36" t="str" cm="1">
+        <f t="array" ref="B36">IF(OR(IF(C36:Z36="X",1,0)),"X","")</f>
+        <v>X</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F36" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="H36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="str" cm="1">
-        <f t="array" ref="B37">IF(OR(IF(C37:Z37="X",1,0)),"X","")</f>
-        <v>X</v>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="H37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38" t="str" cm="1">
-        <f t="array" ref="B38">IF(OR(IF(C38:Z38="X",1,0)),"X","")</f>
-        <v>X</v>
+      <c r="B38" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1376,8 +1463,11 @@
       <c r="G39" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1400,8 +1490,11 @@
       <c r="G40" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1419,7 +1512,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1427,14 +1520,17 @@
         <f t="array" ref="B42">IF(OR(IF(C42:Z42="X",1,0)),"X","")</f>
         <v>X</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="4" t="s">
         <v>62</v>
       </c>
       <c r="G42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1452,7 +1548,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1461,7 +1557,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1484,8 +1580,11 @@
       <c r="G45" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1508,8 +1607,11 @@
       <c r="G46" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1532,8 +1634,11 @@
       <c r="G47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1556,8 +1661,11 @@
       <c r="G48" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1580,8 +1688,11 @@
       <c r="G49" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1604,8 +1715,11 @@
       <c r="G50" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1623,7 +1737,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1632,7 +1746,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1641,7 +1755,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1664,8 +1778,11 @@
       <c r="G54" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1674,7 +1791,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1697,8 +1814,11 @@
       <c r="G56" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1707,7 +1827,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1716,7 +1836,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1725,7 +1845,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1734,7 +1854,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>

</xml_diff>